<commit_message>
Atualização Visual e Funcional do programa
Foi atualizado a apresentação do programa no console e a forma como ele busca o Disco do computador.
</commit_message>
<xml_diff>
--- a/Leitor/bin/ExcelGerado/Infos.xlsx
+++ b/Leitor/bin/ExcelGerado/Infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otonyel Brandão\Desktop\Otonyel\GitHub\LeitorNotebook\Leitor\bin\ExcelGerado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28EB20DE-E56B-4B3B-AF62-DC999C353CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{248D62FE-392F-4FCE-A08C-1E309BE09C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{8174362A-D6C6-45E9-BCD1-E52FFB0B4812}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{579C0CF1-CE8F-4221-8B6A-40CAF5C87232}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações Computador" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>Inspiron 5448</t>
   </si>
   <si>
-    <t>Ok</t>
+    <t>Ativo</t>
   </si>
   <si>
     <t>Seller LEAD</t>
@@ -93,7 +93,7 @@
     <t>11,9 GB</t>
   </si>
   <si>
-    <t>HDD - 931,5 GB</t>
+    <t>SSD 931,5 GB</t>
   </si>
   <si>
     <t>Intel(R) Core(TM) i5-5200U CPU @ 2.20GHz</t>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEDE9FE-5DF0-4448-9BE7-FDAA02853268}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A202757D-1E43-4EEB-88F7-D4B6367BA181}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>